<commit_message>
reset und schön gemacht
</commit_message>
<xml_diff>
--- a/acs_coffee_management/employees_input.xlsx
+++ b/acs_coffee_management/employees_input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lle\workspace\acs-coffee-management\acs_coffee_management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C5AA6AFB-2204-407C-8D7F-4B3CA835501A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2A53607F-00C1-40B4-9C27-3C24279F3FE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="143">
   <si>
     <t>name</t>
   </si>
@@ -55,9 +55,6 @@
     <t>Cazal, Cesar</t>
   </si>
   <si>
-    <t>Chen, Kenny</t>
-  </si>
-  <si>
     <t>Eiling, Niklas</t>
   </si>
   <si>
@@ -76,9 +73,6 @@
     <t>Gier, Wilfried</t>
   </si>
   <si>
-    <t>Hamila, Roua</t>
-  </si>
-  <si>
     <t>Hao, Fenshuo</t>
   </si>
   <si>
@@ -88,12 +82,6 @@
     <t>Hoegen, Marjorie</t>
   </si>
   <si>
-    <t>Joglekar, Charukeshi</t>
-  </si>
-  <si>
-    <t>Josevski, Martina</t>
-  </si>
-  <si>
     <t>Kannan, Yoga</t>
   </si>
   <si>
@@ -112,9 +100,6 @@
     <t>Kröning, Martin</t>
   </si>
   <si>
-    <t>Kumalajati, Arya</t>
-  </si>
-  <si>
     <t>Köster, Iris</t>
   </si>
   <si>
@@ -148,21 +133,12 @@
     <t>Ponci, Ferdinanda</t>
   </si>
   <si>
-    <t>Prein, Simon</t>
-  </si>
-  <si>
     <t>Roth, Lara</t>
   </si>
   <si>
-    <t>Salawudeen, Ahmed</t>
-  </si>
-  <si>
     <t>Sangu, Nagar</t>
   </si>
   <si>
-    <t>Scalabrin, Riccardo</t>
-  </si>
-  <si>
     <t>Schwarz, Sebastian</t>
   </si>
   <si>
@@ -172,12 +148,6 @@
     <t>Sedighi, Foroogh</t>
   </si>
   <si>
-    <t>Simon, Sarah</t>
-  </si>
-  <si>
-    <t>Spies, Emily</t>
-  </si>
-  <si>
     <t>Stoyanova, Ivelina</t>
   </si>
   <si>
@@ -187,24 +157,12 @@
     <t>Tun, Su Mon</t>
   </si>
   <si>
-    <t>Van Megen, Arian</t>
-  </si>
-  <si>
-    <t>Vogel, Steffen</t>
-  </si>
-  <si>
-    <t>Vossel, Christian</t>
-  </si>
-  <si>
     <t>Wege, Felix</t>
   </si>
   <si>
     <t>Wehrmeister, Katharina</t>
   </si>
   <si>
-    <t>Yannik, Jünke</t>
-  </si>
-  <si>
     <t>Yavuzer, Aytug</t>
   </si>
   <si>
@@ -226,9 +184,6 @@
     <t>cesar-cazal</t>
   </si>
   <si>
-    <t>kenny-chen</t>
-  </si>
-  <si>
     <t>niklas-eiling</t>
   </si>
   <si>
@@ -247,9 +202,6 @@
     <t>wilfried-gier</t>
   </si>
   <si>
-    <t>roua-hamila</t>
-  </si>
-  <si>
     <t>fenshuo-hao</t>
   </si>
   <si>
@@ -259,12 +211,6 @@
     <t>marijorie-hoegen</t>
   </si>
   <si>
-    <t>charukeshi-joglekar</t>
-  </si>
-  <si>
-    <t>martina-josevski</t>
-  </si>
-  <si>
     <t>yoga-kannan</t>
   </si>
   <si>
@@ -283,9 +229,6 @@
     <t>martin-kroning</t>
   </si>
   <si>
-    <t>arya-kumalajati</t>
-  </si>
-  <si>
     <t>iris-koster</t>
   </si>
   <si>
@@ -319,21 +262,12 @@
     <t>ferdinanda-ponci</t>
   </si>
   <si>
-    <t>simon-prein</t>
-  </si>
-  <si>
     <t>lara-roth</t>
   </si>
   <si>
-    <t>ahmed-salawudeen</t>
-  </si>
-  <si>
     <t>nagar-sangu</t>
   </si>
   <si>
-    <t>riccardo-scalabrin</t>
-  </si>
-  <si>
     <t>sebastian-schwarz</t>
   </si>
   <si>
@@ -343,12 +277,6 @@
     <t>foroogh-sedighi</t>
   </si>
   <si>
-    <t>sarah-simon</t>
-  </si>
-  <si>
-    <t>emily-spies</t>
-  </si>
-  <si>
     <t>ivelina-stoyanova</t>
   </si>
   <si>
@@ -358,24 +286,12 @@
     <t>su-mon-tun</t>
   </si>
   <si>
-    <t>arian-van-megen</t>
-  </si>
-  <si>
-    <t>steffen-vogel</t>
-  </si>
-  <si>
-    <t>christian-vossel</t>
-  </si>
-  <si>
     <t>felix-wege</t>
   </si>
   <si>
     <t>katharina-wehrmeister</t>
   </si>
   <si>
-    <t>junke-yannik</t>
-  </si>
-  <si>
     <t>aytug-yavuzer</t>
   </si>
   <si>
@@ -397,9 +313,6 @@
     <t>cesar.cazal@eonerc.rwth-aachen.de</t>
   </si>
   <si>
-    <t>nan</t>
-  </si>
-  <si>
     <t>niklas.eiling@eonerc.rwth-aachen.de</t>
   </si>
   <si>
@@ -511,63 +424,9 @@
     <t>aytug.yavuzer@eonerc.rwth-aachen.de</t>
   </si>
   <si>
-    <t>Dejkam, Rahil</t>
-  </si>
-  <si>
-    <t>rahil-dejkam</t>
-  </si>
-  <si>
-    <t>Direya, Rezeq</t>
-  </si>
-  <si>
-    <t>direya-rezeq</t>
-  </si>
-  <si>
-    <t>Li, Chengyang</t>
-  </si>
-  <si>
-    <t>chengyang-li</t>
-  </si>
-  <si>
-    <t>Ray, Calvin</t>
-  </si>
-  <si>
-    <t>calvin-ray</t>
-  </si>
-  <si>
-    <t>Khodadad, Sina</t>
-  </si>
-  <si>
-    <t>sina-khodadad</t>
-  </si>
-  <si>
-    <t>Wnhang, Le Thi Hong</t>
-  </si>
-  <si>
-    <t>le-thi-hong-wnhang</t>
-  </si>
-  <si>
-    <t>Matthias</t>
-  </si>
-  <si>
-    <t>matthias</t>
-  </si>
-  <si>
-    <t>Vasilopoulos, Panagiotis</t>
-  </si>
-  <si>
-    <t>panagiotis-vasiloupolos</t>
-  </si>
-  <si>
     <t>Nardone, Antonio</t>
   </si>
   <si>
-    <t>Bareiss, Vincent</t>
-  </si>
-  <si>
-    <t>bareiss-vincent</t>
-  </si>
-  <si>
     <t>antonio_nardone</t>
   </si>
   <si>
@@ -581,12 +440,6 @@
   </si>
   <si>
     <t>sreejith.pananchickal@eonerc.rwth-aachen.de</t>
-  </si>
-  <si>
-    <t>Cizmeci, Beyza</t>
-  </si>
-  <si>
-    <t>beyza-cizmeci</t>
   </si>
   <si>
     <t>Sitzia, Davide</t>
@@ -974,10 +827,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F71"/>
+  <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="I53" sqref="I53"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1013,10 +866,10 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="D2" t="s">
-        <v>119</v>
+        <v>91</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -1033,10 +886,10 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="D3" t="s">
-        <v>120</v>
+        <v>92</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -1053,10 +906,10 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="D4" t="s">
-        <v>121</v>
+        <v>93</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -1073,10 +926,10 @@
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="D5" t="s">
-        <v>122</v>
+        <v>94</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -1093,10 +946,10 @@
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="D6" t="s">
-        <v>123</v>
+        <v>95</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -1113,10 +966,10 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="D7" t="s">
-        <v>124</v>
+        <v>96</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -1127,16 +980,16 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="D8" t="s">
-        <v>125</v>
+        <v>97</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -1147,16 +1000,16 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="D9" t="s">
-        <v>126</v>
+        <v>98</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -1167,16 +1020,16 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
         <v>13</v>
       </c>
       <c r="C10" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="D10" t="s">
-        <v>127</v>
+        <v>99</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -1187,16 +1040,16 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
         <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="D11" t="s">
-        <v>128</v>
+        <v>100</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -1207,16 +1060,16 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
         <v>15</v>
       </c>
       <c r="C12" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="D12" t="s">
-        <v>129</v>
+        <v>101</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -1227,16 +1080,16 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
         <v>16</v>
       </c>
       <c r="C13" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="D13" t="s">
-        <v>130</v>
+        <v>102</v>
       </c>
       <c r="E13">
         <v>0</v>
@@ -1247,16 +1100,16 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B14" t="s">
         <v>17</v>
       </c>
       <c r="C14" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="D14" t="s">
-        <v>131</v>
+        <v>103</v>
       </c>
       <c r="E14">
         <v>0</v>
@@ -1267,16 +1120,16 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B15" t="s">
         <v>18</v>
       </c>
       <c r="C15" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="D15" t="s">
-        <v>125</v>
+        <v>104</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -1287,16 +1140,16 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B16" t="s">
         <v>19</v>
       </c>
       <c r="C16" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="D16" t="s">
-        <v>132</v>
+        <v>105</v>
       </c>
       <c r="E16">
         <v>0</v>
@@ -1307,16 +1160,16 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B17" t="s">
         <v>20</v>
       </c>
       <c r="C17" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="D17" t="s">
-        <v>133</v>
+        <v>106</v>
       </c>
       <c r="E17">
         <v>0</v>
@@ -1327,16 +1180,16 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B18" t="s">
         <v>21</v>
       </c>
       <c r="C18" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="D18" t="s">
-        <v>134</v>
+        <v>107</v>
       </c>
       <c r="E18">
         <v>0</v>
@@ -1347,16 +1200,16 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B19" t="s">
         <v>22</v>
       </c>
       <c r="C19" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="D19" t="s">
-        <v>125</v>
+        <v>108</v>
       </c>
       <c r="E19">
         <v>0</v>
@@ -1367,16 +1220,16 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B20" t="s">
         <v>23</v>
       </c>
       <c r="C20" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="D20" t="s">
-        <v>125</v>
+        <v>109</v>
       </c>
       <c r="E20">
         <v>0</v>
@@ -1387,16 +1240,16 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B21" t="s">
         <v>24</v>
       </c>
       <c r="C21" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="D21" t="s">
-        <v>135</v>
+        <v>110</v>
       </c>
       <c r="E21">
         <v>0</v>
@@ -1407,16 +1260,16 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B22" t="s">
         <v>25</v>
       </c>
       <c r="C22" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="D22" t="s">
-        <v>136</v>
+        <v>111</v>
       </c>
       <c r="E22">
         <v>0</v>
@@ -1427,16 +1280,16 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="B23" t="s">
         <v>26</v>
       </c>
       <c r="C23" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="D23" t="s">
-        <v>137</v>
+        <v>112</v>
       </c>
       <c r="E23">
         <v>0</v>
@@ -1447,16 +1300,16 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B24" t="s">
         <v>27</v>
       </c>
       <c r="C24" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="D24" t="s">
-        <v>138</v>
+        <v>113</v>
       </c>
       <c r="E24">
         <v>0</v>
@@ -1467,16 +1320,16 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B25" t="s">
         <v>28</v>
       </c>
       <c r="C25" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="D25" t="s">
-        <v>139</v>
+        <v>114</v>
       </c>
       <c r="E25">
         <v>0</v>
@@ -1487,16 +1340,16 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B26" t="s">
         <v>29</v>
       </c>
       <c r="C26" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="D26" t="s">
-        <v>140</v>
+        <v>115</v>
       </c>
       <c r="E26">
         <v>0</v>
@@ -1507,16 +1360,16 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B27" t="s">
         <v>30</v>
       </c>
       <c r="C27" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="D27" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="E27">
         <v>0</v>
@@ -1527,16 +1380,16 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B28" t="s">
         <v>31</v>
       </c>
       <c r="C28" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="D28" t="s">
-        <v>141</v>
+        <v>117</v>
       </c>
       <c r="E28">
         <v>0</v>
@@ -1547,16 +1400,16 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B29" t="s">
         <v>32</v>
       </c>
       <c r="C29" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="D29" t="s">
-        <v>142</v>
+        <v>118</v>
       </c>
       <c r="E29">
         <v>0</v>
@@ -1567,16 +1420,16 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B30" t="s">
         <v>33</v>
       </c>
       <c r="C30" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="D30" t="s">
-        <v>143</v>
+        <v>119</v>
       </c>
       <c r="E30">
         <v>0</v>
@@ -1587,16 +1440,16 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B31" t="s">
         <v>34</v>
       </c>
       <c r="C31" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="D31" t="s">
-        <v>144</v>
+        <v>120</v>
       </c>
       <c r="E31">
         <v>0</v>
@@ -1607,16 +1460,16 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="B32" t="s">
         <v>35</v>
       </c>
       <c r="C32" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="D32" t="s">
-        <v>145</v>
+        <v>121</v>
       </c>
       <c r="E32">
         <v>0</v>
@@ -1627,16 +1480,16 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B33" t="s">
         <v>36</v>
       </c>
       <c r="C33" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="D33" t="s">
-        <v>146</v>
+        <v>122</v>
       </c>
       <c r="E33">
         <v>0</v>
@@ -1647,16 +1500,16 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="B34" t="s">
         <v>37</v>
       </c>
       <c r="C34" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="D34" t="s">
-        <v>147</v>
+        <v>123</v>
       </c>
       <c r="E34">
         <v>0</v>
@@ -1667,16 +1520,16 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="B35" t="s">
         <v>38</v>
       </c>
       <c r="C35" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="D35" t="s">
-        <v>148</v>
+        <v>124</v>
       </c>
       <c r="E35">
         <v>0</v>
@@ -1687,16 +1540,16 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="B36" t="s">
         <v>39</v>
       </c>
       <c r="C36" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="D36" t="s">
-        <v>149</v>
+        <v>125</v>
       </c>
       <c r="E36">
         <v>0</v>
@@ -1707,16 +1560,16 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="B37" t="s">
         <v>40</v>
       </c>
       <c r="C37" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="D37" t="s">
-        <v>150</v>
+        <v>126</v>
       </c>
       <c r="E37">
         <v>0</v>
@@ -1727,16 +1580,16 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="B38" t="s">
         <v>41</v>
       </c>
       <c r="C38" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="D38" t="s">
-        <v>151</v>
+        <v>127</v>
       </c>
       <c r="E38">
         <v>0</v>
@@ -1747,16 +1600,16 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="B39" t="s">
         <v>42</v>
       </c>
       <c r="C39" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="D39" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="E39">
         <v>0</v>
@@ -1767,16 +1620,16 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="B40" t="s">
         <v>43</v>
       </c>
       <c r="C40" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="D40" t="s">
-        <v>152</v>
+        <v>129</v>
       </c>
       <c r="E40">
         <v>0</v>
@@ -1787,16 +1640,16 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="B41" t="s">
         <v>44</v>
       </c>
       <c r="C41" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="D41" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="E41">
         <v>0</v>
@@ -1807,16 +1660,16 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="B42" t="s">
         <v>45</v>
       </c>
       <c r="C42" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="D42" t="s">
-        <v>153</v>
+        <v>131</v>
       </c>
       <c r="E42">
         <v>0</v>
@@ -1827,16 +1680,16 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="B43" t="s">
         <v>46</v>
       </c>
       <c r="C43" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
       <c r="D43" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="E43">
         <v>0</v>
@@ -1847,16 +1700,16 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="B44" t="s">
         <v>47</v>
       </c>
       <c r="C44" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="D44" t="s">
-        <v>154</v>
+        <v>133</v>
       </c>
       <c r="E44">
         <v>0</v>
@@ -1867,16 +1720,16 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
-        <v>43</v>
+        <v>60</v>
       </c>
       <c r="B45" t="s">
-        <v>48</v>
+        <v>137</v>
       </c>
       <c r="C45" t="s">
-        <v>105</v>
-      </c>
-      <c r="D45" t="s">
-        <v>155</v>
+        <v>138</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>139</v>
       </c>
       <c r="E45">
         <v>0</v>
@@ -1887,16 +1740,16 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
-        <v>44</v>
+        <v>64</v>
       </c>
       <c r="B46" t="s">
-        <v>49</v>
+        <v>140</v>
       </c>
       <c r="C46" t="s">
-        <v>106</v>
-      </c>
-      <c r="D46" t="s">
-        <v>156</v>
+        <v>141</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>142</v>
       </c>
       <c r="E46">
         <v>0</v>
@@ -1907,509 +1760,29 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
-        <v>45</v>
+        <v>66</v>
       </c>
       <c r="B47" t="s">
-        <v>50</v>
+        <v>134</v>
       </c>
       <c r="C47" t="s">
-        <v>107</v>
-      </c>
-      <c r="D47" t="s">
-        <v>125</v>
+        <v>135</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>136</v>
       </c>
       <c r="E47">
         <v>0</v>
       </c>
       <c r="F47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="1">
-        <v>46</v>
-      </c>
-      <c r="B48" t="s">
-        <v>51</v>
-      </c>
-      <c r="C48" t="s">
-        <v>108</v>
-      </c>
-      <c r="D48" t="s">
-        <v>125</v>
-      </c>
-      <c r="E48">
-        <v>0</v>
-      </c>
-      <c r="F48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="1">
-        <v>47</v>
-      </c>
-      <c r="B49" t="s">
-        <v>52</v>
-      </c>
-      <c r="C49" t="s">
-        <v>109</v>
-      </c>
-      <c r="D49" t="s">
-        <v>157</v>
-      </c>
-      <c r="E49">
-        <v>0</v>
-      </c>
-      <c r="F49">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="1">
-        <v>48</v>
-      </c>
-      <c r="B50" t="s">
-        <v>53</v>
-      </c>
-      <c r="C50" t="s">
-        <v>110</v>
-      </c>
-      <c r="D50" t="s">
-        <v>158</v>
-      </c>
-      <c r="E50">
-        <v>0</v>
-      </c>
-      <c r="F50">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="1">
-        <v>49</v>
-      </c>
-      <c r="B51" t="s">
-        <v>54</v>
-      </c>
-      <c r="C51" t="s">
-        <v>111</v>
-      </c>
-      <c r="D51" t="s">
-        <v>159</v>
-      </c>
-      <c r="E51">
-        <v>0</v>
-      </c>
-      <c r="F51">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="1">
-        <v>50</v>
-      </c>
-      <c r="B52" t="s">
-        <v>55</v>
-      </c>
-      <c r="C52" t="s">
-        <v>112</v>
-      </c>
-      <c r="D52" t="s">
-        <v>125</v>
-      </c>
-      <c r="E52">
-        <v>0</v>
-      </c>
-      <c r="F52">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="1">
-        <v>51</v>
-      </c>
-      <c r="B53" t="s">
-        <v>56</v>
-      </c>
-      <c r="C53" t="s">
-        <v>113</v>
-      </c>
-      <c r="D53" t="s">
-        <v>125</v>
-      </c>
-      <c r="E53">
-        <v>0</v>
-      </c>
-      <c r="F53">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="1">
-        <v>52</v>
-      </c>
-      <c r="B54" t="s">
-        <v>57</v>
-      </c>
-      <c r="C54" t="s">
-        <v>114</v>
-      </c>
-      <c r="D54" t="s">
-        <v>125</v>
-      </c>
-      <c r="E54">
-        <v>0</v>
-      </c>
-      <c r="F54">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="1">
-        <v>53</v>
-      </c>
-      <c r="B55" t="s">
-        <v>58</v>
-      </c>
-      <c r="C55" t="s">
-        <v>115</v>
-      </c>
-      <c r="D55" t="s">
-        <v>160</v>
-      </c>
-      <c r="E55">
-        <v>0</v>
-      </c>
-      <c r="F55">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="1">
-        <v>54</v>
-      </c>
-      <c r="B56" t="s">
-        <v>59</v>
-      </c>
-      <c r="C56" t="s">
-        <v>116</v>
-      </c>
-      <c r="D56" t="s">
-        <v>161</v>
-      </c>
-      <c r="E56">
-        <v>0</v>
-      </c>
-      <c r="F56">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="1">
-        <v>55</v>
-      </c>
-      <c r="B57" t="s">
-        <v>60</v>
-      </c>
-      <c r="C57" t="s">
-        <v>117</v>
-      </c>
-      <c r="D57" t="s">
-        <v>125</v>
-      </c>
-      <c r="E57">
-        <v>0</v>
-      </c>
-      <c r="F57">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="1">
-        <v>56</v>
-      </c>
-      <c r="B58" t="s">
-        <v>61</v>
-      </c>
-      <c r="C58" t="s">
-        <v>118</v>
-      </c>
-      <c r="D58" t="s">
-        <v>162</v>
-      </c>
-      <c r="E58">
-        <v>0</v>
-      </c>
-      <c r="F58">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="1">
-        <v>57</v>
-      </c>
-      <c r="B59" t="s">
-        <v>163</v>
-      </c>
-      <c r="C59" t="s">
-        <v>164</v>
-      </c>
-      <c r="D59" t="s">
-        <v>125</v>
-      </c>
-      <c r="E59">
-        <v>0</v>
-      </c>
-      <c r="F59">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="1">
-        <v>58</v>
-      </c>
-      <c r="B60" t="s">
-        <v>165</v>
-      </c>
-      <c r="C60" t="s">
-        <v>166</v>
-      </c>
-      <c r="D60" t="s">
-        <v>125</v>
-      </c>
-      <c r="E60">
-        <v>0</v>
-      </c>
-      <c r="F60">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="1">
-        <v>59</v>
-      </c>
-      <c r="B61" t="s">
-        <v>167</v>
-      </c>
-      <c r="C61" t="s">
-        <v>168</v>
-      </c>
-      <c r="D61" t="s">
-        <v>125</v>
-      </c>
-      <c r="E61">
-        <v>0</v>
-      </c>
-      <c r="F61">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="1">
-        <v>60</v>
-      </c>
-      <c r="B62" t="s">
-        <v>184</v>
-      </c>
-      <c r="C62" t="s">
-        <v>185</v>
-      </c>
-      <c r="D62" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="E62">
-        <v>0</v>
-      </c>
-      <c r="F62">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="1">
-        <v>61</v>
-      </c>
-      <c r="B63" t="s">
-        <v>169</v>
-      </c>
-      <c r="C63" t="s">
-        <v>170</v>
-      </c>
-      <c r="D63" t="s">
-        <v>125</v>
-      </c>
-      <c r="E63">
-        <v>0</v>
-      </c>
-      <c r="F63">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="1">
-        <v>62</v>
-      </c>
-      <c r="B64" t="s">
-        <v>180</v>
-      </c>
-      <c r="C64" t="s">
-        <v>181</v>
-      </c>
-      <c r="D64" t="s">
-        <v>125</v>
-      </c>
-      <c r="E64">
-        <v>0</v>
-      </c>
-      <c r="F64">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="1">
-        <v>63</v>
-      </c>
-      <c r="B65" t="s">
-        <v>171</v>
-      </c>
-      <c r="C65" t="s">
-        <v>172</v>
-      </c>
-      <c r="D65" t="s">
-        <v>125</v>
-      </c>
-      <c r="E65">
-        <v>0</v>
-      </c>
-      <c r="F65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="1">
-        <v>64</v>
-      </c>
-      <c r="B66" t="s">
-        <v>189</v>
-      </c>
-      <c r="C66" t="s">
-        <v>190</v>
-      </c>
-      <c r="D66" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="E66">
-        <v>0</v>
-      </c>
-      <c r="F66">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="1">
-        <v>65</v>
-      </c>
-      <c r="B67" t="s">
-        <v>173</v>
-      </c>
-      <c r="C67" t="s">
-        <v>174</v>
-      </c>
-      <c r="D67" t="s">
-        <v>125</v>
-      </c>
-      <c r="E67">
-        <v>0</v>
-      </c>
-      <c r="F67">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" s="1">
-        <v>66</v>
-      </c>
-      <c r="B68" t="s">
-        <v>179</v>
-      </c>
-      <c r="C68" t="s">
-        <v>182</v>
-      </c>
-      <c r="D68" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="E68">
-        <v>0</v>
-      </c>
-      <c r="F68">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="1">
-        <v>67</v>
-      </c>
-      <c r="B69" t="s">
-        <v>187</v>
-      </c>
-      <c r="C69" t="s">
-        <v>188</v>
-      </c>
-      <c r="D69" t="s">
-        <v>125</v>
-      </c>
-      <c r="E69">
-        <v>0</v>
-      </c>
-      <c r="F69">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="1">
-        <v>68</v>
-      </c>
-      <c r="B70" t="s">
-        <v>175</v>
-      </c>
-      <c r="C70" t="s">
-        <v>176</v>
-      </c>
-      <c r="D70" t="s">
-        <v>125</v>
-      </c>
-      <c r="E70">
-        <v>0</v>
-      </c>
-      <c r="F70">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="1">
-        <v>69</v>
-      </c>
-      <c r="B71" t="s">
-        <v>177</v>
-      </c>
-      <c r="C71" t="s">
-        <v>178</v>
-      </c>
-      <c r="D71" t="s">
-        <v>125</v>
-      </c>
-      <c r="E71">
-        <v>0</v>
-      </c>
-      <c r="F71">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D68" r:id="rId1" xr:uid="{9A695081-A4B9-4877-91FF-ADCB505956E6}"/>
-    <hyperlink ref="D62" r:id="rId2" display="mailto:sreejith.pananchickal@eonerc.rwth-aachen.de" xr:uid="{1AF45BB7-E728-4ED6-A824-515BE34153E3}"/>
-    <hyperlink ref="D66" r:id="rId3" xr:uid="{F9A057C0-5FAE-4C70-B301-C6122BEB551D}"/>
+    <hyperlink ref="D47" r:id="rId1" xr:uid="{9A695081-A4B9-4877-91FF-ADCB505956E6}"/>
+    <hyperlink ref="D45" r:id="rId2" display="mailto:sreejith.pananchickal@eonerc.rwth-aachen.de" xr:uid="{1AF45BB7-E728-4ED6-A824-515BE34153E3}"/>
+    <hyperlink ref="D46" r:id="rId3" xr:uid="{F9A057C0-5FAE-4C70-B301-C6122BEB551D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>